<commit_message>
updated readme, cleaned up minor things in example sciprt, updated excel sheet data
</commit_message>
<xml_diff>
--- a/InputData/10Be_data_CRONUS.xlsx
+++ b/InputData/10Be_data_CRONUS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20385"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r_ott\Dropbox\Richard\Crete\Cretan_fans\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r_ott\Dropbox\Richard\PhD_ETH\matlab\My_36Cl_codes\Postburial_production\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E2605E-CACF-450D-A83B-706D73B5C704}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BD6D7B-4BE7-4BDA-B1E9-D9743745CA24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matlab Postburial" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Matlab Erate corrected model1" sheetId="5" r:id="rId3"/>
     <sheet name="Matlab Erate corrected model2" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -964,9 +964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD2" sqref="AD2"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,10 +1158,10 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2">
-        <v>81.319999999999993</v>
+        <v>80.290000000000006</v>
       </c>
       <c r="AI2">
-        <v>8.3800000000000008</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -1229,10 +1229,10 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3">
-        <v>56.94</v>
+        <v>56.81</v>
       </c>
       <c r="AI3">
-        <v>5.87</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>1.5</v>
       </c>
       <c r="AH4">
-        <v>62.67</v>
+        <v>61.67</v>
       </c>
       <c r="AI4">
         <v>5.98</v>
@@ -2109,7 +2109,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="topRight" activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="2">
-        <v>30141</v>
+        <v>29794</v>
       </c>
       <c r="N2">
         <v>153</v>
@@ -2274,8 +2274,8 @@
       <c r="V2">
         <v>0.1</v>
       </c>
-      <c r="Y2">
-        <v>5472.7164187448998</v>
+      <c r="Y2" s="2">
+        <v>5587.0429566990088</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -2310,7 +2310,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <v>26495</v>
+        <v>25798</v>
       </c>
       <c r="N3">
         <v>153</v>
@@ -2324,8 +2324,8 @@
       <c r="V3">
         <v>0.1</v>
       </c>
-      <c r="Y3">
-        <v>6544.6466673152036</v>
+      <c r="Y3" s="2">
+        <v>6943.8444683042835</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -2360,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>11087</v>
+        <v>10686</v>
       </c>
       <c r="N4">
         <v>153</v>
@@ -2374,8 +2374,8 @@
       <c r="V4">
         <v>0.1</v>
       </c>
-      <c r="Y4">
-        <v>3423.9398359200181</v>
+      <c r="Y4" s="2">
+        <v>3628.9508125627717</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -2410,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>33389.169288005323</v>
+        <v>31815.169288005323</v>
       </c>
       <c r="N5">
         <v>153</v>
@@ -2425,7 +2425,7 @@
         <v>0.1</v>
       </c>
       <c r="Y5" s="2">
-        <v>2228.5034172250239</v>
+        <v>2633.2125779328203</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -2460,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>17527.426325440414</v>
+        <v>15259.426325440414</v>
       </c>
       <c r="N6">
         <v>153</v>
@@ -2475,7 +2475,7 @@
         <v>0.1</v>
       </c>
       <c r="Y6" s="2">
-        <v>2025.4170783218219</v>
+        <v>2388.2039990666008</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="2">
-        <v>58936.734988344331</v>
+        <v>57967.734988344331</v>
       </c>
       <c r="N7">
         <v>153</v>
@@ -2525,7 +2525,7 @@
         <v>0.1</v>
       </c>
       <c r="Y7" s="2">
-        <v>2521.4250667478509</v>
+        <v>2632.6109411047437</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -2560,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="2">
-        <v>25622.288922747248</v>
+        <v>24574.288922747248</v>
       </c>
       <c r="N8">
         <v>153</v>
@@ -2575,7 +2575,7 @@
         <v>0.1</v>
       </c>
       <c r="Y8" s="2">
-        <v>1671.2032419143356</v>
+        <v>1859.7831260082412</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -2594,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="2">
-        <v>30696</v>
+        <v>30460</v>
       </c>
       <c r="N2">
         <v>153</v>
@@ -2760,8 +2760,8 @@
       <c r="V2">
         <v>0.1</v>
       </c>
-      <c r="Y2">
-        <v>5331.9699924136858</v>
+      <c r="Y2" s="2">
+        <v>5389.2597821964382</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -2796,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <v>32131.169288005323</v>
+        <v>33206.169288005323</v>
       </c>
       <c r="N3">
         <v>153</v>
@@ -2811,7 +2811,7 @@
         <v>0.1</v>
       </c>
       <c r="Y3" s="2">
-        <v>2535.0409228617214</v>
+        <v>2274.8053720227599</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>16423.426325440414</v>
+        <v>16551.426325440414</v>
       </c>
       <c r="N4">
         <v>153</v>
@@ -2861,7 +2861,7 @@
         <v>0.1</v>
       </c>
       <c r="Y4" s="2">
-        <v>2254.390237105747</v>
+        <v>2177.8003446500106</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>58191.734988344331</v>
+        <v>58822.734988344331</v>
       </c>
       <c r="N5">
         <v>153</v>
@@ -2911,7 +2911,7 @@
         <v>0.1</v>
       </c>
       <c r="Y5" s="2">
-        <v>2599.7579439679384</v>
+        <v>2540.0402294499991</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -2946,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>24804.288922747248</v>
+        <v>25481.288922747248</v>
       </c>
       <c r="N6">
         <v>153</v>
@@ -2961,7 +2961,7 @@
         <v>0.1</v>
       </c>
       <c r="Y6" s="2">
-        <v>1803.2840252675078</v>
+        <v>1702.0415023685484</v>
       </c>
       <c r="AD6">
         <v>0</v>

</xml_diff>